<commit_message>
typo in allocate capex
</commit_message>
<xml_diff>
--- a/DATA_EN_6/reference/capex_pv_calc_casestudies.xlsx
+++ b/DATA_EN_6/reference/capex_pv_calc_casestudies.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikeroberts/OneDrive - UNSW/python/en/DATA_EN_5/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z5044992\Documents\mainDATA\DATA_EN_5\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{35E77F62-4831-40D2-84E8-DCD5BEBDE065}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{6ECDB067-71BC-E841-95FA-8A6923817EE8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E77F62-4831-40D2-84E8-DCD5BEBDE065}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="740" windowWidth="19420" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9375" yWindow="960" windowWidth="13845" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capex_pv_calc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>pv_cap_id</t>
   </si>
@@ -175,24 +175,6 @@
   </si>
   <si>
     <t>profile based on</t>
-  </si>
-  <si>
-    <t>abb_4</t>
-  </si>
-  <si>
-    <t>abb_6</t>
-  </si>
-  <si>
-    <t>abb_8</t>
-  </si>
-  <si>
-    <t>abb_6m</t>
-  </si>
-  <si>
-    <t>abb_8m</t>
-  </si>
-  <si>
-    <t>abb_4m</t>
   </si>
 </sst>
 </file>
@@ -778,7 +760,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -803,7 +785,6 @@
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1052,13 +1033,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1408,33 +1389,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:H25"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1478,7 +1459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1527,7 +1508,7 @@
         <v>9879.9999999999982</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1583,7 +1564,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1635,7 +1616,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1709,7 +1690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1778,7 +1759,7 @@
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1850,7 +1831,7 @@
         <v>0.90186666666666659</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1925,7 +1906,7 @@
         <v>0.85639999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1999,7 +1980,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2074,7 +2055,7 @@
         <v>0.85639999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2148,7 +2129,7 @@
         <v>0.85639999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2222,7 +2203,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2296,7 +2277,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2368,7 +2349,7 @@
       <c r="U14" s="18"/>
       <c r="V14" s="18"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2442,7 +2423,7 @@
       </c>
       <c r="V15" s="18"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2516,7 +2497,7 @@
       </c>
       <c r="V16" s="18"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2590,7 +2571,7 @@
       </c>
       <c r="V17" s="18"/>
     </row>
-    <row r="18" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2662,7 +2643,7 @@
       </c>
       <c r="V18" s="18"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2692,23 +2673,23 @@
         <v>0.65</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" ref="I19:I22" si="21">C19/B19</f>
+        <f t="shared" ref="I19" si="21">C19/B19</f>
         <v>0.20833333333333334</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19:J22" si="22">VLOOKUP(I19,$O$6:$S$18,4,TRUE)</f>
+        <f t="shared" ref="J19" si="22">VLOOKUP(I19,$O$6:$S$18,4,TRUE)</f>
         <v>1.85</v>
       </c>
       <c r="K19" s="6">
-        <f t="shared" ref="K19:K22" si="23">C19*J19*1000</f>
+        <f t="shared" ref="K19" si="23">C19*J19*1000</f>
         <v>27750</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" ref="L19:L22" si="24">VLOOKUP(I19,$O$6:$S$17,5,TRUE)</f>
+        <f t="shared" ref="L19" si="24">VLOOKUP(I19,$O$6:$S$17,5,TRUE)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="M19" s="3">
-        <f t="shared" ref="M19:M22" si="25">L19*C19*1000</f>
+        <f t="shared" ref="M19" si="25">L19*C19*1000</f>
         <v>16500</v>
       </c>
       <c r="N19" s="1" t="s">
@@ -2721,351 +2702,51 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4</v>
-      </c>
-      <c r="D20" s="19">
-        <f t="shared" ref="D20:D25" si="26">VLOOKUP(C20,$O$6:$V$17,8,TRUE)</f>
-        <v>1.61</v>
-      </c>
-      <c r="E20" s="16">
-        <f t="shared" ref="E20:E22" si="27">C20*D20*1000</f>
-        <v>6440</v>
-      </c>
-      <c r="F20" s="16">
-        <f t="shared" ref="F20:F22" si="28">C20*H20*1000</f>
-        <v>3320</v>
-      </c>
-      <c r="G20" s="16">
-        <v>10</v>
-      </c>
-      <c r="H20" s="16">
-        <f t="shared" ref="H20:H22" si="29">VLOOKUP(C20,$O$6:$S$17,5,TRUE)</f>
-        <v>0.83</v>
-      </c>
-      <c r="I20" s="5" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="3" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="6" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="5" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="3" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>6.6</v>
-      </c>
-      <c r="D21" s="19">
-        <f t="shared" si="26"/>
-        <v>1.44</v>
-      </c>
-      <c r="E21" s="16">
-        <f t="shared" si="27"/>
-        <v>9504</v>
-      </c>
-      <c r="F21" s="16">
-        <f t="shared" si="28"/>
-        <v>4290</v>
-      </c>
-      <c r="G21" s="16">
-        <v>10</v>
-      </c>
-      <c r="H21" s="16">
-        <f t="shared" si="29"/>
-        <v>0.65</v>
-      </c>
-      <c r="I21" s="5" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" s="3" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="6" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="5" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" s="3" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D22" s="19">
-        <f t="shared" si="26"/>
-        <v>1.4</v>
-      </c>
-      <c r="E22" s="16">
-        <f t="shared" si="27"/>
-        <v>12320</v>
-      </c>
-      <c r="F22" s="16">
-        <f t="shared" si="28"/>
-        <v>5720.0000000000009</v>
-      </c>
-      <c r="G22" s="16">
-        <v>10</v>
-      </c>
-      <c r="H22" s="16">
-        <f t="shared" si="29"/>
-        <v>0.65</v>
-      </c>
-      <c r="I22" s="5" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" s="3" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="6" t="e">
-        <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="5" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="3" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4</v>
-      </c>
-      <c r="D23" s="16">
-        <f t="shared" ref="D23:D25" si="30">VLOOKUP(C23,$O$6:$S$17,4,TRUE)</f>
-        <v>1.02</v>
-      </c>
-      <c r="E23" s="16">
-        <f t="shared" ref="E23:E25" si="31">C23*D23*1000</f>
-        <v>4080</v>
-      </c>
-      <c r="F23" s="16">
-        <f t="shared" ref="F23:F25" si="32">C23*H23*1000</f>
-        <v>3320</v>
-      </c>
-      <c r="G23" s="16">
-        <v>10</v>
-      </c>
-      <c r="H23" s="16">
-        <f t="shared" ref="H23:H25" si="33">VLOOKUP(C23,$O$6:$S$17,5,TRUE)</f>
-        <v>0.83</v>
-      </c>
-      <c r="I23" s="5" t="e">
-        <f t="shared" ref="I23:I25" si="34">C23/B23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" s="3" t="e">
-        <f t="shared" ref="J23:J25" si="35">VLOOKUP(I23,$O$6:$S$18,4,TRUE)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" s="6" t="e">
-        <f t="shared" ref="K23:K25" si="36">C23*J23*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23" s="5" t="e">
-        <f t="shared" ref="L23:L25" si="37">VLOOKUP(I23,$O$6:$S$17,5,TRUE)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" s="3" t="e">
-        <f t="shared" ref="M23:M25" si="38">L23*C23*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>6.6</v>
-      </c>
-      <c r="D24" s="16">
-        <f t="shared" si="30"/>
-        <v>0.89</v>
-      </c>
-      <c r="E24" s="16">
-        <f t="shared" si="31"/>
-        <v>5874</v>
-      </c>
-      <c r="F24" s="16">
-        <f t="shared" si="32"/>
-        <v>4290</v>
-      </c>
-      <c r="G24" s="16">
-        <v>10</v>
-      </c>
-      <c r="H24" s="16">
-        <f t="shared" si="33"/>
-        <v>0.65</v>
-      </c>
-      <c r="I24" s="5" t="e">
-        <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J24" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K24" s="6" t="e">
-        <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L24" s="5" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M24" s="3" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D25" s="16">
-        <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="16">
-        <f t="shared" si="31"/>
-        <v>8800</v>
-      </c>
-      <c r="F25" s="16">
-        <f t="shared" si="32"/>
-        <v>5720.0000000000009</v>
-      </c>
-      <c r="G25" s="16">
-        <v>10</v>
-      </c>
-      <c r="H25" s="16">
-        <f t="shared" si="33"/>
-        <v>0.65</v>
-      </c>
-      <c r="I25" s="5" t="e">
-        <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" s="3" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K25" s="6" t="e">
-        <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" s="5" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="3" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="1">
         <v>21.6</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D22" s="22">
         <f>(100/(100-21.6)*72)</f>
         <v>91.836734693877546</v>
       </c>
-      <c r="E28" s="22">
-        <f>0.216*D28</f>
+      <c r="E22" s="22">
+        <f>0.216*D22</f>
         <v>19.836734693877549</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B23" s="1">
         <v>21.6</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C23" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="22">
-        <f>D28*1.5</f>
+      <c r="D23" s="22">
+        <f>D22*1.5</f>
         <v>137.75510204081633</v>
       </c>
-      <c r="E29" s="22">
-        <f>0.216*D29</f>
+      <c r="E23" s="22">
+        <f>0.216*D23</f>
         <v>29.755102040816325</v>
       </c>
     </row>
-    <row r="44" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O44" t="s">
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 6A check calcs
</commit_message>
<xml_diff>
--- a/DATA_EN_6/reference/capex_pv_calc_casestudies.xlsx
+++ b/DATA_EN_6/reference/capex_pv_calc_casestudies.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z5044992\Documents\mainDATA\DATA_EN_5\reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikeroberts/OneDrive - UNSW/python/en/DATA_EN_5/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E77F62-4831-40D2-84E8-DCD5BEBDE065}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{35E77F62-4831-40D2-84E8-DCD5BEBDE065}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{6ECDB067-71BC-E841-95FA-8A6923817EE8}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="960" windowWidth="13845" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="740" windowWidth="19420" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capex_pv_calc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>pv_cap_id</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>profile based on</t>
+  </si>
+  <si>
+    <t>abb_4</t>
+  </si>
+  <si>
+    <t>abb_6</t>
+  </si>
+  <si>
+    <t>abb_8</t>
+  </si>
+  <si>
+    <t>abb_6m</t>
+  </si>
+  <si>
+    <t>abb_8m</t>
+  </si>
+  <si>
+    <t>abb_4m</t>
   </si>
 </sst>
 </file>
@@ -760,7 +778,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -785,6 +803,7 @@
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1033,13 +1052,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1389,33 +1408,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="A23" sqref="A23:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1478,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1508,7 +1527,7 @@
         <v>9879.9999999999982</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1564,7 +1583,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1616,7 +1635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1690,7 +1709,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1759,7 +1778,7 @@
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1831,7 +1850,7 @@
         <v>0.90186666666666659</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1906,7 +1925,7 @@
         <v>0.85639999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1980,7 +1999,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2055,7 +2074,7 @@
         <v>0.85639999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2129,7 +2148,7 @@
         <v>0.85639999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2203,7 +2222,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -2277,7 +2296,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2349,7 +2368,7 @@
       <c r="U14" s="18"/>
       <c r="V14" s="18"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2423,7 +2442,7 @@
       </c>
       <c r="V15" s="18"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2497,7 +2516,7 @@
       </c>
       <c r="V16" s="18"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2571,7 +2590,7 @@
       </c>
       <c r="V17" s="18"/>
     </row>
-    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2643,7 +2662,7 @@
       </c>
       <c r="V18" s="18"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2673,23 +2692,23 @@
         <v>0.65</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" ref="I19" si="21">C19/B19</f>
+        <f t="shared" ref="I19:I22" si="21">C19/B19</f>
         <v>0.20833333333333334</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19" si="22">VLOOKUP(I19,$O$6:$S$18,4,TRUE)</f>
+        <f t="shared" ref="J19:J22" si="22">VLOOKUP(I19,$O$6:$S$18,4,TRUE)</f>
         <v>1.85</v>
       </c>
       <c r="K19" s="6">
-        <f t="shared" ref="K19" si="23">C19*J19*1000</f>
+        <f t="shared" ref="K19:K22" si="23">C19*J19*1000</f>
         <v>27750</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" ref="L19" si="24">VLOOKUP(I19,$O$6:$S$17,5,TRUE)</f>
+        <f t="shared" ref="L19:L22" si="24">VLOOKUP(I19,$O$6:$S$17,5,TRUE)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="M19" s="3">
-        <f t="shared" ref="M19" si="25">L19*C19*1000</f>
+        <f t="shared" ref="M19:M22" si="25">L19*C19*1000</f>
         <v>16500</v>
       </c>
       <c r="N19" s="1" t="s">
@@ -2702,51 +2721,351 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4</v>
+      </c>
+      <c r="D20" s="19">
+        <f t="shared" ref="D20:D25" si="26">VLOOKUP(C20,$O$6:$V$17,8,TRUE)</f>
+        <v>1.61</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" ref="E20:E22" si="27">C20*D20*1000</f>
+        <v>6440</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" ref="F20:F22" si="28">C20*H20*1000</f>
+        <v>3320</v>
+      </c>
+      <c r="G20" s="16">
+        <v>10</v>
+      </c>
+      <c r="H20" s="16">
+        <f t="shared" ref="H20:H22" si="29">VLOOKUP(C20,$O$6:$S$17,5,TRUE)</f>
+        <v>0.83</v>
+      </c>
+      <c r="I20" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="3" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="6" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" s="5" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="3" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="D21" s="19">
+        <f t="shared" si="26"/>
+        <v>1.44</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="27"/>
+        <v>9504</v>
+      </c>
+      <c r="F21" s="16">
+        <f t="shared" si="28"/>
+        <v>4290</v>
+      </c>
+      <c r="G21" s="16">
+        <v>10</v>
+      </c>
+      <c r="H21" s="16">
+        <f t="shared" si="29"/>
+        <v>0.65</v>
+      </c>
+      <c r="I21" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="3" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="6" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L21" s="5" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" s="3" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D22" s="19">
+        <f t="shared" si="26"/>
+        <v>1.4</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="27"/>
+        <v>12320</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="28"/>
+        <v>5720.0000000000009</v>
+      </c>
+      <c r="G22" s="16">
+        <v>10</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" si="29"/>
+        <v>0.65</v>
+      </c>
+      <c r="I22" s="5" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="6" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L22" s="5" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="3" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" ref="D23:D25" si="30">VLOOKUP(C23,$O$6:$S$17,4,TRUE)</f>
+        <v>1.02</v>
+      </c>
+      <c r="E23" s="16">
+        <f t="shared" ref="E23:E25" si="31">C23*D23*1000</f>
+        <v>4080</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" ref="F23:F25" si="32">C23*H23*1000</f>
+        <v>3320</v>
+      </c>
+      <c r="G23" s="16">
+        <v>10</v>
+      </c>
+      <c r="H23" s="16">
+        <f t="shared" ref="H23:H25" si="33">VLOOKUP(C23,$O$6:$S$17,5,TRUE)</f>
+        <v>0.83</v>
+      </c>
+      <c r="I23" s="5" t="e">
+        <f t="shared" ref="I23:I25" si="34">C23/B23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" s="3" t="e">
+        <f t="shared" ref="J23:J25" si="35">VLOOKUP(I23,$O$6:$S$18,4,TRUE)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="6" t="e">
+        <f t="shared" ref="K23:K25" si="36">C23*J23*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L23" s="5" t="e">
+        <f t="shared" ref="L23:L25" si="37">VLOOKUP(I23,$O$6:$S$17,5,TRUE)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="3" t="e">
+        <f t="shared" ref="M23:M25" si="38">L23*C23*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="D24" s="16">
+        <f t="shared" si="30"/>
+        <v>0.89</v>
+      </c>
+      <c r="E24" s="16">
+        <f t="shared" si="31"/>
+        <v>5874</v>
+      </c>
+      <c r="F24" s="16">
+        <f t="shared" si="32"/>
+        <v>4290</v>
+      </c>
+      <c r="G24" s="16">
+        <v>10</v>
+      </c>
+      <c r="H24" s="16">
+        <f t="shared" si="33"/>
+        <v>0.65</v>
+      </c>
+      <c r="I24" s="5" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J24" s="3" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K24" s="6" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L24" s="5" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" s="3" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D25" s="16">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="16">
+        <f t="shared" si="31"/>
+        <v>8800</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" si="32"/>
+        <v>5720.0000000000009</v>
+      </c>
+      <c r="G25" s="16">
+        <v>10</v>
+      </c>
+      <c r="H25" s="16">
+        <f t="shared" si="33"/>
+        <v>0.65</v>
+      </c>
+      <c r="I25" s="5" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" s="3" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K25" s="6" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L25" s="5" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" s="3" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B28" s="1">
         <v>21.6</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C28" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D28" s="22">
         <f>(100/(100-21.6)*72)</f>
         <v>91.836734693877546</v>
       </c>
-      <c r="E22" s="22">
-        <f>0.216*D22</f>
+      <c r="E28" s="22">
+        <f>0.216*D28</f>
         <v>19.836734693877549</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B29" s="1">
         <v>21.6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C29" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="22">
-        <f>D22*1.5</f>
+      <c r="D29" s="22">
+        <f>D28*1.5</f>
         <v>137.75510204081633</v>
       </c>
-      <c r="E23" s="22">
-        <f>0.216*D23</f>
+      <c r="E29" s="22">
+        <f>0.216*D29</f>
         <v>29.755102040816325</v>
       </c>
     </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O38" t="s">
+    <row r="44" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O44" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>